<commit_message>
+ I dont remember
</commit_message>
<xml_diff>
--- a/trunk/language.xlsx
+++ b/trunk/language.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="15345" windowHeight="4755"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="15345" windowHeight="4755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="141">
   <si>
     <t>Id</t>
   </si>
@@ -441,6 +441,12 @@
   </si>
   <si>
     <t>https://www.google.com.vn</t>
+  </si>
+  <si>
+    <t>menu_error_server</t>
+  </si>
+  <si>
+    <t>menu_error_caption</t>
   </si>
 </sst>
 </file>
@@ -921,10 +927,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C40" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -1136,360 +1142,382 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="7" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>44</v>
+        <v>104</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>27</v>
+        <v>105</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
-        <v>127</v>
+        <v>47</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B32" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="12" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>65</v>
+        <v>110</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>68</v>
+        <v>107</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="13" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="13" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="13" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="13" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="13" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="13" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="13" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C43" s="1" t="s">
+      <c r="C45" s="1" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="15" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B49" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C47" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A52" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="B52" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="C50" s="17" t="s">
+      <c r="C52" s="17" t="s">
         <v>138</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B50" r:id="rId1"/>
-    <hyperlink ref="C50" r:id="rId2"/>
+    <hyperlink ref="B52" r:id="rId1"/>
+    <hyperlink ref="C52" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>